<commit_message>
Update Sprint Planning doc and Test Report
</commit_message>
<xml_diff>
--- a/docs/Sprint_Planning_Template.xlsx
+++ b/docs/Sprint_Planning_Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ichatspedu.sharepoint.com/teams/DevOpsforAIoTModuleCreation/Shared Documents/General/Mini Project/AY2220/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SP\doaiot\DCPE_2A_22_Group2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E2BB4E-54C1-4433-BE67-0DAA9378FD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16620" windowHeight="6315"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprints" sheetId="3" r:id="rId1"/>
@@ -20,17 +21,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Product Backlog'!$B$3:$I$32</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>Sprint</t>
   </si>
@@ -148,16 +160,129 @@
   </si>
   <si>
     <t>MST + Term Break</t>
+  </si>
+  <si>
+    <t>Start development on the following:
+- SPmart Web Server (adapting from previous project)
+- LCD menus for SPmart self-checkout
+- Keypad programming for SPmart self-checkout</t>
+  </si>
+  <si>
+    <t>Start development on the following:
+- Camera scanning functions
+- LCD menus and keypad for product scanning
+- Integration with SQL database for Product scanning
+Start integrating the following:
+- LCD Keypad for payment
+- RFID for payment
+Start Testing Containerisation:
+- Create Dockerfile, Docker-Compose &amp; Build Images 
+Finish development on the following:
+- SPmart Web Server 
+- MySQL database</t>
+  </si>
+  <si>
+    <t>Finish development on the following:
+- Product Scanning with Camera
+- Integration with SQL database (and Web Server)
+- Unit Tests with PyTest
+- System Tests
+Complete documents for submission:
+- Video demo
+- SRS doc
+- Sprint Planning
+- Test Report</t>
+  </si>
+  <si>
+    <t>LCD Keypad Basic Functions</t>
+  </si>
+  <si>
+    <t>The basic LCD Keypad works, where Outputs are displayed &amp; Inputs are registered</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PyTest Integration</t>
+  </si>
+  <si>
+    <t>The PyTests shall be complete with all PyTests passing</t>
+  </si>
+  <si>
+    <t>Web Server Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a Software Developer, I need to ensure the Web Server is functioning properly </t>
+  </si>
+  <si>
+    <t>Web Server CRUD works after modifying from previous project</t>
+  </si>
+  <si>
+    <t>As a Hardware Developer, I need to ensure that the LCD and Keypad basic functions work</t>
+  </si>
+  <si>
+    <t>SQL Database Development</t>
+  </si>
+  <si>
+    <t>As Software Developer, I need to define additional tables for the database to meet requirements</t>
+  </si>
+  <si>
+    <t>MySQL database modified to include new requirements</t>
+  </si>
+  <si>
+    <t>Payment Functions</t>
+  </si>
+  <si>
+    <t>As a Hardware Developer, I need to ensure that LCD Keypad and RFID is integrated and functioning</t>
+  </si>
+  <si>
+    <t>Basic payment functions as expected</t>
+  </si>
+  <si>
+    <t>Containerization</t>
+  </si>
+  <si>
+    <t>As a Software developer, I need to containerize all 3 images, and ensure that they can be deployed on the RPI</t>
+  </si>
+  <si>
+    <t>Docker containers built and ran succesfully in RPI</t>
+  </si>
+  <si>
+    <t>As a Hardware Developer, i need to ensure that camera functions as expected</t>
+  </si>
+  <si>
+    <t>Camera can detect barcode in RPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Scanning functions </t>
+  </si>
+  <si>
+    <t>As a Hardware Developer, I have to ensure that camera can detect barcodes and fetch data from database</t>
+  </si>
+  <si>
+    <t>Fetch product from database using camera</t>
+  </si>
+  <si>
+    <t>Database Integration</t>
+  </si>
+  <si>
+    <t>As a Software Developer, I need to ensure Web Server can modify products for self-checkout system in real time</t>
+  </si>
+  <si>
+    <t>As Software Developer, I need to define Unit Tests</t>
+  </si>
+  <si>
+    <t>Product attributes edited in real time is reflected in self checkout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +306,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +363,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -280,11 +430,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -333,6 +498,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -350,7 +527,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -364,14 +541,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -385,7 +562,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -664,24 +841,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="B6" zoomScale="147" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="42.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.3046875" customWidth="1"/>
+    <col min="6" max="6" width="42.69140625" customWidth="1"/>
+    <col min="7" max="7" width="18.69140625" customWidth="1"/>
+    <col min="8" max="8" width="20.84375" customWidth="1"/>
+    <col min="9" max="9" width="16.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:9" x14ac:dyDescent="0.4">
       <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
@@ -701,28 +878,28 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="13">
-        <v>44858</v>
+        <v>45222</v>
       </c>
       <c r="H4" s="13">
         <f>G4+11</f>
-        <v>44869</v>
+        <v>45233</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>33</v>
@@ -730,19 +907,19 @@
       <c r="F5" s="4"/>
       <c r="G5" s="13">
         <f>G4+14</f>
-        <v>44872</v>
+        <v>45236</v>
       </c>
       <c r="H5" s="13">
         <f>G5+11</f>
-        <v>44883</v>
+        <v>45247</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D6" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>34</v>
@@ -750,83 +927,89 @@
       <c r="F6" s="4"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6" si="0">G5+14</f>
-        <v>44886</v>
+        <v>45250</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" ref="H6:H10" si="1">G6+11</f>
-        <v>44897</v>
+        <v>45261</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="18" t="s">
+    <row r="7" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D8" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="G8" s="13">
-        <v>44928</v>
+        <v>45292</v>
       </c>
       <c r="H8" s="13">
         <f>G8+11</f>
-        <v>44939</v>
+        <v>45303</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D9" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="G9" s="13">
         <f>G8+14</f>
-        <v>44942</v>
+        <v>45306</v>
       </c>
       <c r="H9" s="13">
         <f>G9+11</f>
-        <v>44953</v>
+        <v>45317</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D10" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="G10" s="13">
         <f t="shared" ref="G10" si="2">G9+14</f>
-        <v>44956</v>
+        <v>45320</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>44967</v>
+        <v>45331</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -834,33 +1017,25 @@
     <mergeCell ref="D7:I7"/>
   </mergeCells>
   <conditionalFormatting sqref="I4:I6">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"Inactive"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Closed"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I6">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I6">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"Closed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I10">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"Inactive"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:I10">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Active"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:I10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Closed"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Inactive"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -871,7 +1046,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>enum!$H$4:$H$6</xm:f>
           </x14:formula1>
@@ -884,21 +1059,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="47.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="47.53515625" customWidth="1"/>
+    <col min="4" max="4" width="49.84375" customWidth="1"/>
+    <col min="5" max="5" width="41.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:5" ht="23.15" x14ac:dyDescent="0.4">
       <c r="C3" s="10" t="s">
         <v>14</v>
       </c>
@@ -909,102 +1084,102 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1019,28 +1194,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:I103"/>
   <sheetViews>
-    <sheetView zoomScale="122" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="78" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="9.140625" style="7"/>
-    <col min="3" max="3" width="36.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.15234375" style="8"/>
+    <col min="2" max="2" width="9.15234375" style="7"/>
+    <col min="3" max="3" width="36.3046875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="32.53515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="32" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.53515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="14.69140625" style="8" customWidth="1"/>
     <col min="8" max="8" width="15" style="7" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="9" max="9" width="14.3828125" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.15234375" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1066,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="84.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="6">
         <v>1</v>
       </c>
@@ -1086,312 +1261,417 @@
         <v>5</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B5" s="6">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="19">
+        <v>6</v>
+      </c>
+      <c r="G5" s="19">
+        <v>9</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B6" s="6">
         <f t="shared" ref="B6:B69" si="0">B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2</v>
+      </c>
+      <c r="G6" s="19">
+        <v>2</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B7" s="6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="19">
+        <v>2</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B8" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="19">
+        <v>5</v>
+      </c>
+      <c r="G8" s="19">
+        <v>5</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="19">
+        <v>5</v>
+      </c>
+      <c r="G9" s="19">
+        <v>18</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="19">
+        <v>1</v>
+      </c>
+      <c r="G10" s="19">
+        <v>3</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B11" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="19">
+        <v>3</v>
+      </c>
+      <c r="G11" s="19">
+        <v>1</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="58.3" x14ac:dyDescent="0.4">
       <c r="B12" s="6">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="19">
+        <v>3</v>
+      </c>
+      <c r="G12" s="19">
+        <v>2</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B13" s="6">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="19">
+        <v>1</v>
+      </c>
+      <c r="G13" s="19">
+        <v>1</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B14" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B16" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" s="6">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" s="6">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="6">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="6">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B23" s="6">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" s="6">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" s="6">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1404,7 +1684,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B29" s="6">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1417,7 +1697,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B30" s="6">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1430,7 +1710,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B31" s="6">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1443,7 +1723,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" s="6">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1456,7 +1736,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B33" s="6">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1469,7 +1749,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B34" s="6">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1482,7 +1762,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B35" s="6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1495,7 +1775,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B36" s="6">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1508,7 +1788,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B37" s="6">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1521,7 +1801,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B38" s="6">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1534,7 +1814,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B39" s="6">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1547,7 +1827,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B40" s="6">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1560,7 +1840,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B41" s="6">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1573,7 +1853,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B42" s="6">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1586,7 +1866,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B43" s="6">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1599,7 +1879,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B44" s="6">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1612,7 +1892,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B45" s="6">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1625,7 +1905,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B46" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1638,7 +1918,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B47" s="6">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1651,7 +1931,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B48" s="6">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1664,7 +1944,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B49" s="6">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1677,7 +1957,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B50" s="6">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1690,7 +1970,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B51" s="6">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1703,7 +1983,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B52" s="6">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1716,7 +1996,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B53" s="6">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1729,7 +2009,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B54" s="6">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1742,7 +2022,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B55" s="6">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1755,7 +2035,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B56" s="6">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1768,7 +2048,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B57" s="6">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1781,7 +2061,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B58" s="6">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1794,7 +2074,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B59" s="6">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1807,7 +2087,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B60" s="6">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1820,7 +2100,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B61" s="6">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1833,7 +2113,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B62" s="6">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1846,7 +2126,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B63" s="6">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1859,7 +2139,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B64" s="6">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1872,7 +2152,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B65" s="6">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1885,7 +2165,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B66" s="6">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1898,7 +2178,7 @@
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
     </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B67" s="6">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1911,7 +2191,7 @@
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
     </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B68" s="6">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1924,7 +2204,7 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
     </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B69" s="6">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1937,7 +2217,7 @@
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
     </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B70" s="6">
         <f t="shared" ref="B70:B103" si="1">B69+1</f>
         <v>67</v>
@@ -1950,7 +2230,7 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B71" s="6">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -1963,7 +2243,7 @@
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B72" s="6">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1976,7 +2256,7 @@
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B73" s="6">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1989,7 +2269,7 @@
       <c r="H73" s="6"/>
       <c r="I73" s="6"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B74" s="6">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -2002,7 +2282,7 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B75" s="6">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -2015,7 +2295,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B76" s="6">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2028,7 +2308,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B77" s="6">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2041,7 +2321,7 @@
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B78" s="6">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -2054,7 +2334,7 @@
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B79" s="6">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -2067,7 +2347,7 @@
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B80" s="6">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -2080,7 +2360,7 @@
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B81" s="6">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -2093,7 +2373,7 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B82" s="6">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -2106,7 +2386,7 @@
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B83" s="6">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2119,7 +2399,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B84" s="6">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -2132,7 +2412,7 @@
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B85" s="6">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -2145,7 +2425,7 @@
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B86" s="6">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -2158,7 +2438,7 @@
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B87" s="6">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -2171,7 +2451,7 @@
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B88" s="6">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -2184,7 +2464,7 @@
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B89" s="6">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -2197,7 +2477,7 @@
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B90" s="6">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -2210,7 +2490,7 @@
       <c r="H90" s="6"/>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B91" s="6">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -2223,7 +2503,7 @@
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B92" s="6">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -2236,7 +2516,7 @@
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B93" s="6">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -2249,7 +2529,7 @@
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B94" s="6">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -2262,7 +2542,7 @@
       <c r="H94" s="6"/>
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B95" s="6">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -2275,7 +2555,7 @@
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B96" s="6">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -2288,7 +2568,7 @@
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B97" s="6">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -2301,7 +2581,7 @@
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B98" s="6">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -2316,7 +2596,7 @@
       </c>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B99" s="6">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -2329,7 +2609,7 @@
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B100" s="6">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -2342,7 +2622,7 @@
       <c r="H100" s="6"/>
       <c r="I100" s="6"/>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B101" s="6">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -2355,7 +2635,7 @@
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B102" s="6">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -2368,7 +2648,7 @@
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B103" s="6">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2382,7 +2662,7 @@
       <c r="I103" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:I32"/>
+  <autoFilter ref="B3:I32" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2391,17 +2671,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>enum!$B$4:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>I4:I103</xm:sqref>
+          <xm:sqref>I4 I28:I103</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>enum!$F$4:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H4:H103</xm:sqref>
+          <xm:sqref>H4 H28:H103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2410,20 +2690,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2440,7 +2720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -2451,7 +2731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -2462,7 +2742,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -2473,17 +2753,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>12</v>
       </c>

</xml_diff>